<commit_message>
added check for additional samples and expanded model
</commit_message>
<xml_diff>
--- a/dist/solverdportal.xlsx
+++ b/dist/solverdportal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcruvolo/Github/projects-solve-rd/dist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591E66BE-6988-8740-8FFA-C41654EB463C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD0EF08-45D9-7C49-85AE-9067F1CD4123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31160" yWindow="-1440" windowWidth="27640" windowHeight="16760" activeTab="3" xr2:uid="{6D9E4540-5669-5745-AFC0-E6D9361D7C59}"/>
+    <workbookView xWindow="-31160" yWindow="-1440" windowWidth="27640" windowHeight="16760" activeTab="2" xr2:uid="{6D9E4540-5669-5745-AFC0-E6D9361D7C59}"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="90">
   <si>
     <t>name</t>
   </si>
@@ -303,6 +303,12 @@
   </si>
   <si>
     <t>conflicting seq type</t>
+  </si>
+  <si>
+    <t>sample_id2</t>
+  </si>
+  <si>
+    <t>Combined virtual samples and novelomics IDs</t>
   </si>
 </sst>
 </file>
@@ -759,10 +765,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869F885-D5EB-4F46-862B-D3299A512E61}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="28.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -845,10 +851,10 @@
         <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -859,10 +865,10 @@
         <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
         <v>31</v>
@@ -873,10 +879,10 @@
         <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
         <v>31</v>
@@ -887,7 +893,10 @@
         <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
       </c>
       <c r="D7" t="s">
         <v>31</v>
@@ -898,7 +907,7 @@
         <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
         <v>31</v>
@@ -909,7 +918,7 @@
         <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
         <v>31</v>
@@ -920,7 +929,7 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
         <v>31</v>
@@ -931,10 +940,7 @@
         <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
         <v>31</v>
@@ -945,7 +951,10 @@
         <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
       </c>
       <c r="D12" t="s">
         <v>31</v>
@@ -956,7 +965,7 @@
         <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
         <v>31</v>
@@ -967,16 +976,10 @@
         <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" t="b">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -984,13 +987,16 @@
         <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
-      </c>
-      <c r="I15" t="s">
-        <v>50</v>
+        <v>37</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -998,10 +1004,13 @@
         <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>45</v>
+      </c>
+      <c r="I16" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1009,16 +1018,10 @@
         <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1026,16 +1029,13 @@
         <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" t="b">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
       </c>
       <c r="H18" t="s">
         <v>42</v>
@@ -1043,16 +1043,22 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" t="b">
+        <v>36</v>
+      </c>
+      <c r="F19" t="b">
         <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1060,9 +1066,23 @@
         <v>50</v>
       </c>
       <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
         <v>2</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1075,7 +1095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0078841-CB42-F641-925E-D4A0FF46C2A7}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: added summary counts dataset
</commit_message>
<xml_diff>
--- a/dist/solverdportal.xlsx
+++ b/dist/solverdportal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcruvolo/Github/projects-solve-rd/dist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B37C385-F34B-504E-A285-1C8605E3F92C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACBD908-6083-244F-9D58-5AD8A7353769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31160" yWindow="-1440" windowWidth="27640" windowHeight="16760" activeTab="3" xr2:uid="{6D9E4540-5669-5745-AFC0-E6D9361D7C59}"/>
+    <workbookView xWindow="-31160" yWindow="-1440" windowWidth="25200" windowHeight="12980" xr2:uid="{6D9E4540-5669-5745-AFC0-E6D9361D7C59}"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="104">
   <si>
     <t>name</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Solve-RD Portal</t>
   </si>
   <si>
-    <t>New official datatransfers from GPAP, CNAG (v0.9)</t>
-  </si>
-  <si>
     <t>package</t>
   </si>
   <si>
@@ -333,6 +330,27 @@
   </si>
   <si>
     <t>there is no ERN value to validate</t>
+  </si>
+  <si>
+    <t>solverdportal_experiment_counts</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>experiment_counts</t>
+  </si>
+  <si>
+    <t>GPAP Experiment Counts</t>
+  </si>
+  <si>
+    <t>Summary of errors</t>
+  </si>
+  <si>
+    <t>New official datatransfers from GPAP, CNAG (v0.91)</t>
   </si>
 </sst>
 </file>
@@ -686,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4398441C-5EE7-7F40-9B4E-BA97159EB081}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -716,7 +734,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -726,10 +744,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E33A890-4BD7-CA47-8466-57376B7DF13F}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -751,18 +769,18 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -770,15 +788,29 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
         <v>47</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>48</v>
       </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
       <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -789,10 +821,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869F885-D5EB-4F46-862B-D3299A512E61}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="28.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -809,7 +841,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -818,39 +850,39 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
-        <v>33</v>
-      </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -858,177 +890,177 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
         <v>88</v>
       </c>
-      <c r="C4" t="s">
-        <v>89</v>
-      </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" t="s">
         <v>94</v>
       </c>
-      <c r="C12" t="s">
-        <v>95</v>
-      </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G16" t="b">
         <v>0</v>
@@ -1039,75 +1071,75 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
         <v>44</v>
       </c>
-      <c r="D17" t="s">
-        <v>45</v>
-      </c>
       <c r="I17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
         <v>39</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G19" t="b">
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
         <v>34</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>35</v>
-      </c>
-      <c r="D20" t="s">
-        <v>36</v>
       </c>
       <c r="F20" t="b">
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E21" t="b">
         <v>1</v>
@@ -1115,13 +1147,49 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1133,7 +1201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0078841-CB42-F641-925E-D4A0FF46C2A7}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -1153,170 +1221,170 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" t="s">
         <v>92</v>
-      </c>
-      <c r="B3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" t="s">
         <v>96</v>
-      </c>
-      <c r="B10" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" t="s">
         <v>90</v>
-      </c>
-      <c r="B11" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
         <v>61</v>
-      </c>
-      <c r="B16" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" t="s">
         <v>72</v>
-      </c>
-      <c r="B17" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
         <v>66</v>
-      </c>
-      <c r="B19" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: restructured files; added gpap reporting script; updated model
</commit_message>
<xml_diff>
--- a/dist/solverdportal.xlsx
+++ b/dist/solverdportal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcruvolo/Github/projects-solve-rd/dist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACBD908-6083-244F-9D58-5AD8A7353769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C193BDF-369D-A14F-9C44-4096405C2381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31160" yWindow="-1440" windowWidth="25200" windowHeight="12980" xr2:uid="{6D9E4540-5669-5745-AFC0-E6D9361D7C59}"/>
+    <workbookView xWindow="-31160" yWindow="-1440" windowWidth="25200" windowHeight="12980" activeTab="2" xr2:uid="{6D9E4540-5669-5745-AFC0-E6D9361D7C59}"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="109">
   <si>
     <t>name</t>
   </si>
@@ -351,6 +351,21 @@
   </si>
   <si>
     <t>New official datatransfers from GPAP, CNAG (v0.91)</t>
+  </si>
+  <si>
+    <t>record_url</t>
+  </si>
+  <si>
+    <t>aggregate_url</t>
+  </si>
+  <si>
+    <t>hyperlink</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -704,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4398441C-5EE7-7F40-9B4E-BA97159EB081}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -821,10 +836,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869F885-D5EB-4F46-862B-D3299A512E61}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="28.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1190,6 +1205,39 @@
       </c>
       <c r="D25" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>